<commit_message>
My Summoners can be persistently checked
</commit_message>
<xml_diff>
--- a/Art/Color_calc.xlsx
+++ b/Art/Color_calc.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="5">
         <f>0.75*D11</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E10" s="5">
         <f>0.75*E11</f>
@@ -604,7 +604,7 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="1"/>
@@ -619,7 +619,9 @@
         <f>C10/0.75</f>
         <v>0</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="13">
+        <v>24</v>
+      </c>
       <c r="E11" s="8">
         <f>E12/1.5</f>
         <v>0</v>
@@ -630,7 +632,7 @@
       </c>
       <c r="G11" s="8">
         <f>G14/3</f>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="H11" s="9">
         <f>H15/4</f>
@@ -647,7 +649,7 @@
       </c>
       <c r="D12" s="8">
         <f>1.5*D11</f>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="8">
@@ -656,7 +658,7 @@
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="2"/>
@@ -673,7 +675,7 @@
       </c>
       <c r="D13" s="8">
         <f>2*D11</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E13" s="8">
         <f>2*E11</f>
@@ -681,8 +683,8 @@
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="8">
-        <f t="shared" ref="F13:H13" si="3">2*G11</f>
-        <v>112</v>
+        <f t="shared" ref="G13:H13" si="3">2*G11</f>
+        <v>0</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="3"/>
@@ -699,7 +701,7 @@
       </c>
       <c r="D14" s="8">
         <f>3*D11</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="E14" s="8">
         <f>3*E11</f>
@@ -709,9 +711,7 @@
         <f t="shared" ref="F14:H14" si="4">3*F11</f>
         <v>0</v>
       </c>
-      <c r="G14" s="13">
-        <v>168</v>
-      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -727,19 +727,19 @@
       </c>
       <c r="D15" s="11">
         <f>4*D11</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E15" s="11">
         <f>4*E11</f>
         <v>0</v>
       </c>
       <c r="F15" s="11">
-        <f t="shared" ref="F15:H15" si="5">4*F11</f>
+        <f t="shared" ref="F15:G15" si="5">4*F11</f>
         <v>0</v>
       </c>
       <c r="G15" s="11">
         <f t="shared" si="5"/>
-        <v>224</v>
+        <v>0</v>
       </c>
       <c r="H15" s="14"/>
     </row>

</xml_diff>

<commit_message>
icons (only) in the bottom navigation
</commit_message>
<xml_diff>
--- a/Art/Color_calc.xlsx
+++ b/Art/Color_calc.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="5">
         <f>0.75*D11</f>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E10" s="5">
         <f>0.75*E11</f>
@@ -604,7 +604,7 @@
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6">
         <f t="shared" si="1"/>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="13">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E11" s="8">
         <f>E12/1.5</f>
@@ -632,7 +632,7 @@
       </c>
       <c r="G11" s="8">
         <f>G14/3</f>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="H11" s="9">
         <f>H15/4</f>
@@ -649,7 +649,7 @@
       </c>
       <c r="D12" s="8">
         <f>1.5*D11</f>
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="8">
@@ -658,7 +658,7 @@
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="2"/>
@@ -675,7 +675,7 @@
       </c>
       <c r="D13" s="8">
         <f>2*D11</f>
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E13" s="8">
         <f>2*E11</f>
@@ -684,7 +684,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="8">
         <f t="shared" ref="G13:H13" si="3">2*G11</f>
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="3"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="D14" s="8">
         <f>3*D11</f>
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="E14" s="8">
         <f>3*E11</f>
@@ -711,9 +711,7 @@
         <f t="shared" ref="F14:H14" si="4">3*F11</f>
         <v>0</v>
       </c>
-      <c r="G14" s="13">
-        <v>168</v>
-      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="9">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -729,7 +727,7 @@
       </c>
       <c r="D15" s="11">
         <f>4*D11</f>
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="E15" s="11">
         <f>4*E11</f>
@@ -741,7 +739,7 @@
       </c>
       <c r="G15" s="11">
         <f t="shared" si="5"/>
-        <v>224</v>
+        <v>0</v>
       </c>
       <c r="H15" s="14"/>
     </row>

</xml_diff>